<commit_message>
Update layout.xlsx from desktop uploader
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Shared With Me\4. RME-P\intern\06 - Projects\2026 eInk Displays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC168BF-5505-4B48-BF72-4838CBEA6827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55426955-E704-4305-AA03-BD593769F16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20115" yWindow="-16935" windowWidth="14445" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="1160" windowWidth="14400" windowHeight="8920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -404,13 +404,13 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -443,7 +443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>

</xml_diff>